<commit_message>
Added report paper to git folder
</commit_message>
<xml_diff>
--- a/PolicyTestingData.xlsx
+++ b/PolicyTestingData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REU Internship\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REU Internship\Git stuff\Other GPMS\GPMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1544,7 +1544,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1647,8 +1647,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1665,6 +1672,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1792,10 +1804,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1964,6 +1977,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1979,20 +2004,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2273,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2292,7 +2309,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="65" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -2310,7 +2327,7 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="24" t="s">
         <v>16</v>
       </c>
@@ -2371,28 +2388,28 @@
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3488,7 +3505,7 @@
       <c r="J47" s="8"/>
     </row>
     <row r="48" spans="1:10" ht="240" x14ac:dyDescent="0.2">
-      <c r="A48" s="33">
+      <c r="A48" s="67">
         <v>38</v>
       </c>
       <c r="B48" s="32" t="s">
@@ -4255,75 +4272,75 @@
     </row>
     <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="11"/>
-      <c r="B93" s="63"/>
+      <c r="B93" s="58"/>
       <c r="C93" s="11"/>
-      <c r="D93" s="64"/>
-      <c r="E93" s="64"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="59"/>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
-      <c r="I93" s="63"/>
-      <c r="J93" s="65"/>
+      <c r="I93" s="58"/>
+      <c r="J93" s="60"/>
     </row>
     <row r="94" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="11"/>
-      <c r="B94" s="63"/>
+      <c r="B94" s="58"/>
       <c r="C94" s="11"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
+      <c r="D94" s="59"/>
+      <c r="E94" s="59"/>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
-      <c r="I94" s="63"/>
-      <c r="J94" s="65"/>
+      <c r="I94" s="58"/>
+      <c r="J94" s="60"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="66"/>
-      <c r="B95" s="66"/>
-      <c r="C95" s="66"/>
+      <c r="A95" s="61"/>
+      <c r="B95" s="61"/>
+      <c r="C95" s="61"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
-      <c r="I95" s="63"/>
-      <c r="J95" s="65"/>
+      <c r="I95" s="58"/>
+      <c r="J95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="11"/>
-      <c r="B96" s="63"/>
+      <c r="B96" s="58"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="65"/>
+      <c r="I96" s="58"/>
+      <c r="J96" s="60"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="11"/>
-      <c r="B97" s="63"/>
+      <c r="B97" s="58"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
-      <c r="I97" s="63"/>
-      <c r="J97" s="65"/>
+      <c r="I97" s="58"/>
+      <c r="J97" s="60"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="11"/>
-      <c r="B98" s="63"/>
+      <c r="B98" s="58"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
-      <c r="I98" s="63"/>
-      <c r="J98" s="65"/>
+      <c r="I98" s="58"/>
+      <c r="J98" s="60"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="18"/>

</xml_diff>